<commit_message>
- updated IE Driver to v3.12.0.4. - added new System variable - `nexial.web.preemptiveAlertCheck` - to opt out for pre-emptive checks of `alert`,   `confirm` or `prompt` (JavaScript) dialogs during web automation. This pre-emptive checks are turned on by default   for convenience.  However for performance reason one might opt to turn off this check (which DOES take time), esp.   when automating a web app that does not generate JavaScript dialog (`alert`, `confirm` or `prompt`). Our simple tests   show that switching this System variable to `false` (default is `true`) yields about 15-20% time improvement.   - note that if this System variable is set to `true` or undefined, any harvested alert text would be available via the     `nexial.lastAlertTet` System variable. - code fix to avoid exception in [web &raquo; `selectWindowByIndex(index)`](../commands/web/selectWindowByIndex(index))
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/data/web-showcase.data.xlsx
+++ b/src/test/resources/showcase/artifact/data/web-showcase.data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/showcase/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5731E8C0-BFE4-9148-9D4A-BD27455250EB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D09F60A-F708-A243-B019-21D1EF467F1F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="20480" windowHeight="12540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="48">
   <si>
     <t>true</t>
   </si>
@@ -203,54 +203,6 @@
   </si>
   <si>
     <t>Nexial</t>
-  </si>
-  <si>
-    <t>nexial.notifyOnExecutionStart</t>
-  </si>
-  <si>
-    <t>nexial.notifyOnExecutionComplete</t>
-  </si>
-  <si>
-    <t>nexial.notifyOnScriptStart</t>
-  </si>
-  <si>
-    <t>nexial.notifyOnScriptComplete</t>
-  </si>
-  <si>
-    <t>nexial.notifyOnScenarioStart</t>
-  </si>
-  <si>
-    <t>nexial.notifyOnScenarioComplete</t>
-  </si>
-  <si>
-    <t>nexial.notifyOnError</t>
-  </si>
-  <si>
-    <t>nexial.notifyOnPause</t>
-  </si>
-  <si>
-    <t>tts:execution start</t>
-  </si>
-  <si>
-    <t>tts:execution complete</t>
-  </si>
-  <si>
-    <t>tts:script start</t>
-  </si>
-  <si>
-    <t>tts:script complete</t>
-  </si>
-  <si>
-    <t>tts:scenario start</t>
-  </si>
-  <si>
-    <t>tts:scenario complete</t>
-  </si>
-  <si>
-    <t>tts:error found</t>
-  </si>
-  <si>
-    <t>tts:execution pause</t>
   </si>
 </sst>
 </file>
@@ -1276,10 +1228,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AAA20"/>
+  <dimension ref="A1:AAA12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -1400,71 +1352,7 @@
         <v>45</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:703">
-      <c r="A13" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="14" spans="1:703">
-      <c r="A14" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="15" spans="1:703">
-      <c r="A15" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="16" spans="1:703">
-      <c r="A16" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>63</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- output spreadsheet now include link to multiple log files. - when `nexial.outputToCloud` is set to `true`, Nexial wil re-upload log files to S3 towards the end of the execution   so that the log file will have nearly the complete log information. - fixed error that was preventing execution summary (JSON) to be uploaded to cloud storage.
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/data/web-showcase.data.xlsx
+++ b/src/test/resources/showcase/artifact/data/web-showcase.data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/showcase/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D09F60A-F708-A243-B019-21D1EF467F1F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A31B5FC5-14F4-AC4C-9168-62BAC9576649}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="20480" windowHeight="12540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,7 +46,7 @@
     <definedName name="ws">'[1]#system'!$P$2:$P$15</definedName>
     <definedName name="xml">'[1]#system'!$O$2:$O$12</definedName>
   </definedNames>
-  <calcPr calcId="150000"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="48">
   <si>
     <t>true</t>
   </si>
@@ -1228,10 +1228,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AAA12"/>
+  <dimension ref="A1:AAA13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -1352,7 +1352,15 @@
         <v>45</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:703">
+      <c r="A13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- generates JUnit-compatible XML at the end of execution. This file is **ALWAYS** named as `junit.xml` and placed in   the output directory. - console output now includes additional information useful for CI/CD. - fixed issue when running different browser between iterations or scripts (within plan).
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/data/web-showcase.data.xlsx
+++ b/src/test/resources/showcase/artifact/data/web-showcase.data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10115"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/showcase/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F52E7FE8-0D92-834A-A091-1473E431D225}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA670219-A0DD-0945-BB9B-5AC30F2410D2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="20480" windowHeight="12540" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="51200" windowHeight="10520" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -20,9 +20,10 @@
     <sheet name="amazon" sheetId="7" r:id="rId5"/>
     <sheet name="exec_script" sheetId="8" r:id="rId6"/>
     <sheet name="http_basic" sheetId="9" r:id="rId7"/>
+    <sheet name="mobile_emulation" sheetId="10" r:id="rId8"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId8"/>
+    <externalReference r:id="rId9"/>
   </externalReferences>
   <definedNames>
     <definedName name="base">'[1]#system'!$B$2:$B$24</definedName>
@@ -47,7 +48,7 @@
     <definedName name="ws">'[1]#system'!$P$2:$P$15</definedName>
     <definedName name="xml">'[1]#system'!$O$2:$O$12</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179017" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -60,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="62">
   <si>
     <t>true</t>
   </si>
@@ -204,6 +205,48 @@
   </si>
   <si>
     <t>Nexial</t>
+  </si>
+  <si>
+    <t>nexial.browser.emulation.userAgent</t>
+  </si>
+  <si>
+    <t>nexial.browser.emulation.width</t>
+  </si>
+  <si>
+    <t>nexial.browser.emulation.height</t>
+  </si>
+  <si>
+    <t>Mozilla/5.0 (iPhone; CPU iPhone OS 11_0 like Mac OS X) AppleWebKit/604.1.38 (KHTML, like Gecko) Version/11.0 Mobile/15A372 Safari/604.1</t>
+  </si>
+  <si>
+    <t>iPhone X</t>
+  </si>
+  <si>
+    <t>site.url</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com</t>
+  </si>
+  <si>
+    <t>site.footer.signinLink</t>
+  </si>
+  <si>
+    <t>css=#nav-ftr-auth</t>
+  </si>
+  <si>
+    <t>emulationDeviceTarget</t>
+  </si>
+  <si>
+    <t>414</t>
+  </si>
+  <si>
+    <t>736</t>
+  </si>
+  <si>
+    <t>site.footer2</t>
+  </si>
+  <si>
+    <t>css=#navBackToTop</t>
   </si>
 </sst>
 </file>
@@ -353,7 +396,72 @@
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="50">
+  <dxfs count="55">
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1432,21 +1540,21 @@
   </sheetData>
   <sheetProtection sheet="1" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="beginsWith" dxfId="49" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="54" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="48" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="53" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="47" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="52" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="46" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="51" priority="4" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="45" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="50" priority="5">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1586,21 +1694,21 @@
   </sheetData>
   <sheetProtection sheet="1" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="beginsWith" dxfId="44" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="49" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="43" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="48" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="42" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="47" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="41" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="46" priority="4" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="40" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="45" priority="5">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1740,29 +1848,29 @@
   </sheetData>
   <sheetProtection sheet="1" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="beginsWith" dxfId="39" priority="5" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="44" priority="5" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="38" priority="6" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="43" priority="6" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="37" priority="7" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="42" priority="7" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B9 B11:B1048576">
-    <cfRule type="expression" dxfId="36" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="41" priority="8" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="35" priority="9">
+    <cfRule type="notContainsBlanks" dxfId="40" priority="9">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="expression" dxfId="34" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="1" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="33" priority="2">
+    <cfRule type="notContainsBlanks" dxfId="38" priority="2">
       <formula>LEN(TRIM(B10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1837,40 +1945,40 @@
   </sheetData>
   <sheetProtection sheet="1" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A8:A1048576 A2:A6">
-    <cfRule type="beginsWith" dxfId="32" priority="6" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="37" priority="6" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A2,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="31" priority="7" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="36" priority="7" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A2,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="30" priority="8" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="35" priority="8" stopIfTrue="1">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B1048576 B2:B6">
-    <cfRule type="expression" dxfId="29" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="28" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="33" priority="10">
       <formula>LEN(TRIM(B2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="beginsWith" dxfId="27" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="32" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="26" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="31" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="25" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="30" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1">
-    <cfRule type="expression" dxfId="24" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="4" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="23" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="28" priority="5">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2014,51 +2122,51 @@
   </sheetData>
   <sheetProtection sheet="1" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A4:A1048576 A1">
-    <cfRule type="beginsWith" dxfId="22" priority="9" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="27" priority="9" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="21" priority="10" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="26" priority="10" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="20" priority="11" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="25" priority="11" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4 B1 B6:B1048576">
-    <cfRule type="expression" dxfId="19" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="12" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="18" priority="13">
+    <cfRule type="notContainsBlanks" dxfId="23" priority="13">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="beginsWith" dxfId="17" priority="4" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="22" priority="4" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A2,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="16" priority="5" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="21" priority="5" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A2,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="15" priority="6" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="20" priority="6" stopIfTrue="1">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="expression" dxfId="14" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="7" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="13" priority="8">
+    <cfRule type="notContainsBlanks" dxfId="18" priority="8">
       <formula>LEN(TRIM(B2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3">
-    <cfRule type="beginsWith" dxfId="12" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="17" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A3,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="11" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="16" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A3,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="10" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="15" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A3))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2185,21 +2293,21 @@
   </sheetData>
   <sheetProtection sheet="1" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="beginsWith" dxfId="9" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="14" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="8" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="13" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="7" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="12" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="6" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="4" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="5" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="10" priority="5">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2212,7 +2320,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD25EFE1-04CC-A449-AAE0-0807648F1AB2}">
   <dimension ref="A1:AAA10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -2318,21 +2426,151 @@
   </sheetData>
   <sheetProtection sheet="1" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="beginsWith" dxfId="4" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="9" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="3" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="8" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="2" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="7" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="1" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="4" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="5" priority="5">
+      <formula>LEN(TRIM(B1))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{245CE3E3-6AD2-7B46-9205-5D48456750E8}">
+  <dimension ref="A1:AAA10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
+  <cols>
+    <col min="1" max="1" width="33.1640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.1640625" style="2" customWidth="1" collapsed="1"/>
+    <col min="3" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:703">
+      <c r="A1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="HA1" s="7"/>
+      <c r="AAA1" s="7"/>
+    </row>
+    <row r="2" spans="1:703">
+      <c r="A2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="HA2" s="7"/>
+      <c r="AAA2" s="7"/>
+    </row>
+    <row r="3" spans="1:703">
+      <c r="A3" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="HA3" s="7"/>
+      <c r="AAA3" s="7"/>
+    </row>
+    <row r="4" spans="1:703">
+      <c r="A4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="HA4" s="4"/>
+      <c r="AAA4" s="5"/>
+    </row>
+    <row r="5" spans="1:703">
+      <c r="A5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="HA5" s="4"/>
+      <c r="AAA5" s="5"/>
+    </row>
+    <row r="6" spans="1:703">
+      <c r="A6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="HA6" s="4"/>
+      <c r="AAA6" s="5"/>
+    </row>
+    <row r="7" spans="1:703">
+      <c r="A7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="HA7" s="4"/>
+      <c r="AAA7" s="5"/>
+    </row>
+    <row r="8" spans="1:703">
+      <c r="A8" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="HA8" s="4"/>
+      <c r="AAA8" s="5"/>
+    </row>
+    <row r="9" spans="1:703">
+      <c r="HA9" s="4"/>
+      <c r="AAA9" s="5"/>
+    </row>
+    <row r="10" spans="1:703">
+      <c r="HA10" s="4"/>
+      <c r="AAA10" s="5"/>
+    </row>
+  </sheetData>
+  <sheetProtection insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
+  <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="beginsWith" dxfId="2" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="1" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="4" priority="3" stopIfTrue="1">
+      <formula>LEN(TRIM(A1))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="expression" dxfId="0" priority="4" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="3" priority="5">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
[improvements] - removed `java.awt.headless=true` from .commons.sh in order to support Robot-based type key
[desktop]
- [`typeKeys`]: *NEW* command to automate a series of `keystrokes` to the current execution environment.

Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/data/web-showcase.data.xlsx
+++ b/src/test/resources/showcase/artifact/data/web-showcase.data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10115"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10530"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/showcase/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA670219-A0DD-0945-BB9B-5AC30F2410D2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC5E50D1-0BC3-684C-9CBF-4695B8AB2AB9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="51200" windowHeight="10520" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="10520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -48,7 +48,7 @@
     <definedName name="ws">'[1]#system'!$P$2:$P$15</definedName>
     <definedName name="xml">'[1]#system'!$O$2:$O$12</definedName>
   </definedNames>
-  <calcPr calcId="179017" concurrentCalc="0"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="64">
   <si>
     <t>true</t>
   </si>
@@ -247,6 +247,12 @@
   </si>
   <si>
     <t>css=#navBackToTop</t>
+  </si>
+  <si>
+    <t>9555</t>
+  </si>
+  <si>
+    <t>//nexial.browser.chrome.remote.port</t>
   </si>
 </sst>
 </file>
@@ -399,6 +405,20 @@
   <dxfs count="55">
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
         <i/>
         <strike val="0"/>
@@ -415,6 +435,18 @@
       <font>
         <b/>
         <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
         <color theme="4" tint="-0.24994659260841701"/>
       </font>
       <fill>
@@ -433,32 +465,6 @@
       <fill>
         <patternFill>
           <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <u val="none"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1402,10 +1408,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AAA13"/>
+  <dimension ref="A1:AAA14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -1535,6 +1541,14 @@
       </c>
       <c r="B13" s="2" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:703">
+      <c r="A14" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -2453,8 +2467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{245CE3E3-6AD2-7B46-9205-5D48456750E8}">
   <dimension ref="A1:AAA10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -2556,21 +2570,21 @@
   </sheetData>
   <sheetProtection insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="beginsWith" dxfId="2" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="4" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="3" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="4" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="2" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="0" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="4" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "nexial.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="3" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="5">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
[web] - use ChromeDriverService so that chrome driver can reuse same port for driver-browser communication. This helps to   stabilize chrome browser automation.
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/data/web-showcase.data.xlsx
+++ b/src/test/resources/showcase/artifact/data/web-showcase.data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/showcase/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC5E50D1-0BC3-684C-9CBF-4695B8AB2AB9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CED6BFA-912D-3042-A999-1538457B42F8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="10520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15760" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -48,7 +48,7 @@
     <definedName name="ws">'[1]#system'!$P$2:$P$15</definedName>
     <definedName name="xml">'[1]#system'!$O$2:$O$12</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179017" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="65">
   <si>
     <t>true</t>
   </si>
@@ -141,9 +141,6 @@
     <t>productBrand</t>
   </si>
   <si>
-    <t>Seiko Watches</t>
-  </si>
-  <si>
     <t>productReview</t>
   </si>
   <si>
@@ -153,18 +150,9 @@
     <t>mostExpense.title</t>
   </si>
   <si>
-    <t>SEIKO ProspEx diver scuba titanium solar reverse rotation prevention bezel black SBDN001 men's watch</t>
-  </si>
-  <si>
     <t>mostExpense.startPrice</t>
   </si>
   <si>
-    <t>$10,010</t>
-  </si>
-  <si>
-    <t>1,612</t>
-  </si>
-  <si>
     <t>2000</t>
   </si>
   <si>
@@ -252,7 +240,22 @@
     <t>9555</t>
   </si>
   <si>
-    <t>//nexial.browser.chrome.remote.port</t>
+    <t>nexial.browser.logChrome</t>
+  </si>
+  <si>
+    <t>nexial.browser.chrome.remote.port</t>
+  </si>
+  <si>
+    <t>SEIKO</t>
+  </si>
+  <si>
+    <t>$5,200</t>
+  </si>
+  <si>
+    <t>Seiko Mens ASTRON GPS Limited Edition Solar Watch, SSE060</t>
+  </si>
+  <si>
+    <t>796</t>
   </si>
 </sst>
 </file>
@@ -1408,10 +1411,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AAA14"/>
+  <dimension ref="A1:AAA15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -1424,7 +1427,7 @@
   <sheetData>
     <row r="1" spans="1:703">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>3</v>
@@ -1432,7 +1435,7 @@
     </row>
     <row r="2" spans="1:703">
       <c r="A2" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -1442,7 +1445,7 @@
     </row>
     <row r="3" spans="1:703">
       <c r="A3" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>4</v>
@@ -1452,14 +1455,14 @@
     </row>
     <row r="4" spans="1:703">
       <c r="A4" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="HA4" s="7"/>
       <c r="AAA4" s="7"/>
     </row>
     <row r="5" spans="1:703">
       <c r="A5" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>6</v>
@@ -1469,7 +1472,7 @@
     </row>
     <row r="6" spans="1:703">
       <c r="A6" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>5</v>
@@ -1479,7 +1482,7 @@
     </row>
     <row r="7" spans="1:703">
       <c r="A7" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>1</v>
@@ -1489,7 +1492,7 @@
     </row>
     <row r="8" spans="1:703">
       <c r="A8" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>2</v>
@@ -1499,7 +1502,7 @@
     </row>
     <row r="9" spans="1:703">
       <c r="A9" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>0</v>
@@ -1512,7 +1515,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="HA10" s="4"/>
       <c r="AAA10" s="5"/>
@@ -1529,7 +1532,7 @@
     </row>
     <row r="12" spans="1:703">
       <c r="A12" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>11</v>
@@ -1537,7 +1540,7 @@
     </row>
     <row r="13" spans="1:703">
       <c r="A13" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>0</v>
@@ -1545,10 +1548,18 @@
     </row>
     <row r="14" spans="1:703">
       <c r="A14" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:703">
+      <c r="A15" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1596,7 +1607,7 @@
   <sheetData>
     <row r="1" spans="1:703">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>3</v>
@@ -1604,7 +1615,7 @@
     </row>
     <row r="2" spans="1:703">
       <c r="A2" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -1614,7 +1625,7 @@
     </row>
     <row r="3" spans="1:703">
       <c r="A3" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>13</v>
@@ -1624,14 +1635,14 @@
     </row>
     <row r="4" spans="1:703">
       <c r="A4" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="HA4" s="7"/>
       <c r="AAA4" s="7"/>
     </row>
     <row r="5" spans="1:703">
       <c r="A5" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>6</v>
@@ -1641,7 +1652,7 @@
     </row>
     <row r="6" spans="1:703">
       <c r="A6" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>5</v>
@@ -1651,7 +1662,7 @@
     </row>
     <row r="7" spans="1:703">
       <c r="A7" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>1</v>
@@ -1661,7 +1672,7 @@
     </row>
     <row r="8" spans="1:703">
       <c r="A8" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>2</v>
@@ -1671,7 +1682,7 @@
     </row>
     <row r="9" spans="1:703">
       <c r="A9" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>0</v>
@@ -1681,7 +1692,7 @@
     </row>
     <row r="10" spans="1:703">
       <c r="A10" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>12</v>
@@ -1697,7 +1708,7 @@
     </row>
     <row r="11" spans="1:703">
       <c r="A11" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>5</v>
@@ -1750,7 +1761,7 @@
   <sheetData>
     <row r="1" spans="1:703">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>3</v>
@@ -1758,7 +1769,7 @@
     </row>
     <row r="2" spans="1:703">
       <c r="A2" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -1768,7 +1779,7 @@
     </row>
     <row r="3" spans="1:703">
       <c r="A3" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>4</v>
@@ -1778,14 +1789,14 @@
     </row>
     <row r="4" spans="1:703">
       <c r="A4" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="HA4" s="7"/>
       <c r="AAA4" s="7"/>
     </row>
     <row r="5" spans="1:703">
       <c r="A5" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>6</v>
@@ -1795,7 +1806,7 @@
     </row>
     <row r="6" spans="1:703">
       <c r="A6" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>5</v>
@@ -1805,7 +1816,7 @@
     </row>
     <row r="7" spans="1:703">
       <c r="A7" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>1</v>
@@ -1815,7 +1826,7 @@
     </row>
     <row r="8" spans="1:703">
       <c r="A8" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>2</v>
@@ -1825,7 +1836,7 @@
     </row>
     <row r="9" spans="1:703">
       <c r="A9" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>0</v>
@@ -1835,7 +1846,7 @@
     </row>
     <row r="10" spans="1:703">
       <c r="A10" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>10</v>
@@ -1851,7 +1862,7 @@
     </row>
     <row r="11" spans="1:703">
       <c r="A11" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>5</v>
@@ -1909,7 +1920,7 @@
   <sheetData>
     <row r="1" spans="1:703">
       <c r="A1" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -2005,8 +2016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AAA12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -2019,7 +2030,7 @@
   <sheetData>
     <row r="1" spans="1:703">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>4</v>
@@ -2027,7 +2038,7 @@
     </row>
     <row r="2" spans="1:703">
       <c r="A2" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
@@ -2090,7 +2101,7 @@
         <v>24</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="HA8" s="4"/>
       <c r="AAA8" s="5"/>
@@ -2100,37 +2111,37 @@
         <v>25</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="HA9" s="4"/>
       <c r="AAA9" s="5"/>
     </row>
     <row r="10" spans="1:703">
       <c r="A10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="HA10" s="4"/>
       <c r="AAA10" s="5"/>
     </row>
     <row r="11" spans="1:703">
       <c r="A11" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>30</v>
+        <v>63</v>
       </c>
       <c r="HA11" s="4"/>
       <c r="AAA11" s="5"/>
     </row>
     <row r="12" spans="1:703">
       <c r="A12" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>32</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -2207,7 +2218,7 @@
   <sheetData>
     <row r="1" spans="1:703">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>3</v>
@@ -2215,7 +2226,7 @@
     </row>
     <row r="2" spans="1:703">
       <c r="A2" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -2225,7 +2236,7 @@
     </row>
     <row r="3" spans="1:703">
       <c r="A3" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>4</v>
@@ -2235,24 +2246,24 @@
     </row>
     <row r="4" spans="1:703">
       <c r="A4" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="HA4" s="7"/>
       <c r="AAA4" s="7"/>
     </row>
     <row r="5" spans="1:703">
       <c r="A5" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="HA5" s="4"/>
       <c r="AAA5" s="5"/>
     </row>
     <row r="6" spans="1:703">
       <c r="A6" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>5</v>
@@ -2262,17 +2273,17 @@
     </row>
     <row r="7" spans="1:703">
       <c r="A7" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="HA7" s="4"/>
       <c r="AAA7" s="5"/>
     </row>
     <row r="8" spans="1:703">
       <c r="A8" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>2</v>
@@ -2282,7 +2293,7 @@
     </row>
     <row r="9" spans="1:703">
       <c r="A9" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>0</v>
@@ -2292,7 +2303,7 @@
     </row>
     <row r="10" spans="1:703">
       <c r="A10" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>11</v>
@@ -2348,7 +2359,7 @@
   <sheetData>
     <row r="1" spans="1:703">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -2358,7 +2369,7 @@
     </row>
     <row r="2" spans="1:703">
       <c r="A2" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
@@ -2368,24 +2379,24 @@
     </row>
     <row r="3" spans="1:703">
       <c r="A3" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="HA3" s="7"/>
       <c r="AAA3" s="7"/>
     </row>
     <row r="4" spans="1:703">
       <c r="A4" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="HA4" s="4"/>
       <c r="AAA4" s="5"/>
     </row>
     <row r="5" spans="1:703">
       <c r="A5" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>5</v>
@@ -2395,17 +2406,17 @@
     </row>
     <row r="6" spans="1:703">
       <c r="A6" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="HA6" s="4"/>
       <c r="AAA6" s="5"/>
     </row>
     <row r="7" spans="1:703">
       <c r="A7" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>2</v>
@@ -2415,7 +2426,7 @@
     </row>
     <row r="8" spans="1:703">
       <c r="A8" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>0</v>
@@ -2425,7 +2436,7 @@
     </row>
     <row r="9" spans="1:703">
       <c r="A9" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>11</v>
@@ -2481,7 +2492,7 @@
   <sheetData>
     <row r="1" spans="1:703">
       <c r="A1" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>11</v>
@@ -2491,70 +2502,70 @@
     </row>
     <row r="2" spans="1:703">
       <c r="A2" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="HA2" s="7"/>
       <c r="AAA2" s="7"/>
     </row>
     <row r="3" spans="1:703">
       <c r="A3" s="6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="HA3" s="7"/>
       <c r="AAA3" s="7"/>
     </row>
     <row r="4" spans="1:703">
       <c r="A4" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="HA4" s="4"/>
       <c r="AAA4" s="5"/>
     </row>
     <row r="5" spans="1:703">
       <c r="A5" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="HA5" s="4"/>
       <c r="AAA5" s="5"/>
     </row>
     <row r="6" spans="1:703">
       <c r="A6" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="HA6" s="4"/>
       <c r="AAA6" s="5"/>
     </row>
     <row r="7" spans="1:703">
       <c r="A7" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="HA7" s="4"/>
       <c r="AAA7" s="5"/>
     </row>
     <row r="8" spans="1:703">
       <c r="A8" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="HA8" s="4"/>
       <c r="AAA8" s="5"/>

</xml_diff>